<commit_message>
Add Name.trim() into the code,Name can be compared without space at the
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/wineprice/Tarif Formats 2016 Duclot Export.xlsx
+++ b/src/main/webapp/WEB-INF/wineprice/Tarif Formats 2016 Duclot Export.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesHo\wildfly-8.2.1.Final\standalone\deployments\comparewine.war\WEB-INF\wineprice\"/>
     </mc:Choice>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3500" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="318">
   <si>
     <t>Pomerol</t>
   </si>
@@ -1002,6 +1002,15 @@
   <si>
     <t>CROIX DE BEAUCAILLOU GRANDE RESERVE</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price Euro</t>
+  </si>
+  <si>
+    <t>Bottle Size</t>
+  </si>
 </sst>
 </file>
 
@@ -1013,7 +1022,7 @@
   <fonts count="22">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1042,14 +1051,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
@@ -1082,20 +1091,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="36"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1116,32 +1125,32 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="48"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="36"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="28"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Tw Cen MT"/>
       <family val="2"/>
     </font>
@@ -1174,7 +1183,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4487,16 +4496,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="35.75" style="13" customWidth="1"/>
-    <col min="2" max="2" width="23.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="26.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="7.625" style="8" customWidth="1"/>
-    <col min="9" max="255" width="11.375" style="1" customWidth="1"/>
-    <col min="256" max="16384" width="0.125" style="1" hidden="1"/>
+    <col min="1" max="1" customWidth="true" style="13" width="35.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="23.625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="13.375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="10.625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="10.625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="26.125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="8" width="22.875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="8" width="7.625" collapsed="true"/>
+    <col min="9" max="255" customWidth="true" style="1" width="11.375" collapsed="true"/>
+    <col min="256" max="16384" hidden="true" style="1" width="0.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="15" spans="1:7" ht="15" customHeight="1">
@@ -4559,7 +4568,7 @@
     <row r="26" spans="1:7" ht="42.75" customHeight="1"/>
     <row r="80" spans="1:9" s="57" customFormat="1" ht="15">
       <c r="A80" s="45" t="s">
-        <v>153</v>
+        <v>315</v>
       </c>
       <c r="B80" s="45" t="s">
         <v>154</v>
@@ -4571,13 +4580,13 @@
         <v>156</v>
       </c>
       <c r="E80" s="46" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
       <c r="F80" s="45" t="s">
         <v>157</v>
       </c>
       <c r="G80" s="47" t="s">
-        <v>151</v>
+        <v>317</v>
       </c>
       <c r="H80" s="47" t="s">
         <v>165</v>
@@ -32012,9 +32021,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32026,9 +32035,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId2"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32040,9 +32049,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId3"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32054,9 +32063,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId4"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32068,9 +32077,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId5"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32082,9 +32091,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId6"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32096,9 +32105,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" r:id="rId7"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32110,9 +32119,9 @@
       <printOptions horizontalCentered="1"/>
       <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId8"/>
       <headerFooter>
-        <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+        <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
         <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
       </headerFooter>
@@ -32128,9 +32137,9 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="1.6535433070866143" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="portrait" r:id="rId9"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;C&amp;G
-&amp;"Tw Cen MT,Normal"&amp;14Tarif Format - Duclot Export&amp;"-,Normal"&amp;11
-</oddHeader>
+    <oddHeader xml:space="preserve"><![CDATA[&C&G
+&"Tw Cen MT,Normal"&14Tarif Format - Duclot Export&"-,Normal"&11
+]]></oddHeader>
     <oddFooter>&amp;CPRICES IN EURO EX CELLARS BORDEAUX - SUBJECT TO AVAILIBILITY
 Page &amp;P de &amp;N</oddFooter>
   </headerFooter>

</xml_diff>